<commit_message>
quase chegando ao objetivo da consolidação
</commit_message>
<xml_diff>
--- a/planilas-mari-weg/TIN Collaboration.xlsx
+++ b/planilas-mari-weg/TIN Collaboration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://weg365.sharepoint.com/teams/BR-TI-TIN/Alocacao Recursos/TIN - Detalhamento Atividades/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\consolidar-planilha-weg\planilas-mari-weg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3720" documentId="13_ncr:1_{4B5C97CF-A05B-44F9-AB64-DCE1104D12C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DA1A3E7-E108-4A04-A3DB-E1618A3616ED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456F4D28-4594-43E8-B1DD-48252D4C9F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2985" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -808,7 +808,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -900,58 +900,59 @@
     <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bom" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Ênfase1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="318">
+  <dxfs count="241">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -973,6 +974,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC4D79B"/>
@@ -988,6 +1009,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF538DD5"/>
         </patternFill>
       </fill>
@@ -1013,6 +1055,12 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF538DD5"/>
@@ -1358,10 +1406,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1378,6 +1427,19 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC4D79B"/>
@@ -1385,10 +1447,31 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1398,6 +1481,19 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC5D9F1"/>
@@ -1407,15 +1503,23 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC4D79B"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1425,6 +1529,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC5D9F1"/>
@@ -1432,6 +1556,18 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC4D79B"/>
@@ -1439,10 +1575,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1452,6 +1589,19 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC5D9F1"/>
@@ -1466,10 +1616,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1479,693 +1637,10 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2808,149 +2283,149 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3B6310A3-E34A-4CD5-A7FB-2FA909562852}" name="Tabela13" displayName="Tabela13" ref="A1:T23" totalsRowShown="0" headerRowDxfId="317" dataDxfId="316">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3B6310A3-E34A-4CD5-A7FB-2FA909562852}" name="Tabela13" displayName="Tabela13" ref="A1:T23" totalsRowShown="0" headerRowDxfId="240" dataDxfId="239">
   <autoFilter ref="A1:T23" xr:uid="{60C5897C-4C10-4DE1-B6BC-B05ADF30BE1F}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{8B1A9690-2E27-4A0C-9DF6-7CC6B2DC87ED}" name="Epic" dataDxfId="315"/>
-    <tableColumn id="2" xr3:uid="{8C272838-9FA9-4BBC-BBCE-3EC8C12101CB}" name="Ações" dataDxfId="314"/>
-    <tableColumn id="16" xr3:uid="{E354EF09-D61B-4DAF-98AB-0B0614B0A98B}" name="Status" dataDxfId="313"/>
-    <tableColumn id="3" xr3:uid="{2AABEEB5-A12C-4DE2-8248-978A0DC4D3E5}" name="Due Date" dataDxfId="312"/>
-    <tableColumn id="4" xr3:uid="{0C75C268-AE5C-4E82-B76B-2ADB807A0365}" name="Assignee" dataDxfId="311"/>
-    <tableColumn id="23" xr3:uid="{BC236957-04A8-4FEC-8204-F7BD5F4969A4}" name="Estimated effort" dataDxfId="310"/>
-    <tableColumn id="5" xr3:uid="{D504A01F-D1AF-4F01-96AE-65ED703556D5}" name="Planned effort" dataDxfId="309">
+    <tableColumn id="1" xr3:uid="{8B1A9690-2E27-4A0C-9DF6-7CC6B2DC87ED}" name="Epic" dataDxfId="238"/>
+    <tableColumn id="2" xr3:uid="{8C272838-9FA9-4BBC-BBCE-3EC8C12101CB}" name="Ações" dataDxfId="237"/>
+    <tableColumn id="16" xr3:uid="{E354EF09-D61B-4DAF-98AB-0B0614B0A98B}" name="Status" dataDxfId="236"/>
+    <tableColumn id="3" xr3:uid="{2AABEEB5-A12C-4DE2-8248-978A0DC4D3E5}" name="Due Date" dataDxfId="235"/>
+    <tableColumn id="4" xr3:uid="{0C75C268-AE5C-4E82-B76B-2ADB807A0365}" name="Assignee" dataDxfId="234"/>
+    <tableColumn id="23" xr3:uid="{BC236957-04A8-4FEC-8204-F7BD5F4969A4}" name="Estimated effort" dataDxfId="233"/>
+    <tableColumn id="5" xr3:uid="{D504A01F-D1AF-4F01-96AE-65ED703556D5}" name="Planned effort" dataDxfId="232">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{758C47E5-C839-4201-B5C8-1D9F00604F19}" name="Mês 1" dataDxfId="308"/>
-    <tableColumn id="7" xr3:uid="{567F833B-87CB-49E3-BDB8-79F26D8F2730}" name="Mês 2" dataDxfId="307"/>
-    <tableColumn id="8" xr3:uid="{981B754C-7BB7-470F-8014-AF4B50817565}" name="Mês 3" dataDxfId="306"/>
-    <tableColumn id="9" xr3:uid="{1C18D282-B6B5-4FC5-835A-A867DEC4ADF6}" name="Mês 4" dataDxfId="305"/>
-    <tableColumn id="10" xr3:uid="{D4E3BF5E-F46D-4805-80AA-2A64E74EDD02}" name="Mês 5" dataDxfId="304"/>
-    <tableColumn id="11" xr3:uid="{04F1CD94-15F9-4DB6-9FC1-84FC0564EBC0}" name="Mês 6" dataDxfId="303"/>
-    <tableColumn id="12" xr3:uid="{68B6B203-AA78-4FA0-BD80-DC0AB82F5DDD}" name="Mês 7" dataDxfId="302"/>
-    <tableColumn id="13" xr3:uid="{2C15EBEF-5293-4B87-A96B-78CBB1DD85A2}" name="Mês 8" dataDxfId="301"/>
-    <tableColumn id="14" xr3:uid="{B9CB2FC4-87A3-4262-9BA5-5249DC68E7BF}" name="Mês 9" dataDxfId="300"/>
-    <tableColumn id="15" xr3:uid="{214F1BAC-DA30-4A8D-B437-640434011392}" name="Mês 10" dataDxfId="299"/>
-    <tableColumn id="22" xr3:uid="{5D3DFDD0-4A2A-451B-9336-B6071B70243D}" name="Mês 11" dataDxfId="298"/>
-    <tableColumn id="21" xr3:uid="{B37F580D-6E8B-4963-944B-5E949A64FC4A}" name="Mês 12" dataDxfId="297"/>
-    <tableColumn id="20" xr3:uid="{5F2CA737-F580-43E6-8D75-2539F9B103D0}" name="Nota" dataDxfId="296"/>
+    <tableColumn id="6" xr3:uid="{758C47E5-C839-4201-B5C8-1D9F00604F19}" name="Mês 1" dataDxfId="231"/>
+    <tableColumn id="7" xr3:uid="{567F833B-87CB-49E3-BDB8-79F26D8F2730}" name="Mês 2" dataDxfId="230"/>
+    <tableColumn id="8" xr3:uid="{981B754C-7BB7-470F-8014-AF4B50817565}" name="Mês 3" dataDxfId="229"/>
+    <tableColumn id="9" xr3:uid="{1C18D282-B6B5-4FC5-835A-A867DEC4ADF6}" name="Mês 4" dataDxfId="228"/>
+    <tableColumn id="10" xr3:uid="{D4E3BF5E-F46D-4805-80AA-2A64E74EDD02}" name="Mês 5" dataDxfId="227"/>
+    <tableColumn id="11" xr3:uid="{04F1CD94-15F9-4DB6-9FC1-84FC0564EBC0}" name="Mês 6" dataDxfId="226"/>
+    <tableColumn id="12" xr3:uid="{68B6B203-AA78-4FA0-BD80-DC0AB82F5DDD}" name="Mês 7" dataDxfId="225"/>
+    <tableColumn id="13" xr3:uid="{2C15EBEF-5293-4B87-A96B-78CBB1DD85A2}" name="Mês 8" dataDxfId="224"/>
+    <tableColumn id="14" xr3:uid="{B9CB2FC4-87A3-4262-9BA5-5249DC68E7BF}" name="Mês 9" dataDxfId="223"/>
+    <tableColumn id="15" xr3:uid="{214F1BAC-DA30-4A8D-B437-640434011392}" name="Mês 10" dataDxfId="222"/>
+    <tableColumn id="22" xr3:uid="{5D3DFDD0-4A2A-451B-9336-B6071B70243D}" name="Mês 11" dataDxfId="221"/>
+    <tableColumn id="21" xr3:uid="{B37F580D-6E8B-4963-944B-5E949A64FC4A}" name="Mês 12" dataDxfId="220"/>
+    <tableColumn id="20" xr3:uid="{5F2CA737-F580-43E6-8D75-2539F9B103D0}" name="Nota" dataDxfId="219"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1487AFAB-D12A-487F-9815-C3DDF17D25E9}" name="Tabela1456725" displayName="Tabela1456725" ref="A1:Z32" totalsRowShown="0" headerRowDxfId="295" dataDxfId="294">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1487AFAB-D12A-487F-9815-C3DDF17D25E9}" name="Tabela1456725" displayName="Tabela1456725" ref="A1:Z32" totalsRowShown="0" headerRowDxfId="218" dataDxfId="217">
   <autoFilter ref="A1:Z32" xr:uid="{60C5897C-4C10-4DE1-B6BC-B05ADF30BE1F}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{01209A68-7F85-4C28-AFB5-81C5B0EC7A37}" name="Epic" dataDxfId="293"/>
-    <tableColumn id="2" xr3:uid="{66517A9E-46E1-41DF-9F0B-17AB54123296}" name="Ações" dataDxfId="292"/>
-    <tableColumn id="16" xr3:uid="{92F7750A-D683-45B5-80BF-2568989D936C}" name="Status" dataDxfId="291"/>
-    <tableColumn id="3" xr3:uid="{67DDF4A4-1CB4-4009-BCDB-046B5F84434E}" name="Due Date" dataDxfId="290"/>
-    <tableColumn id="4" xr3:uid="{CA9093F9-48BC-4FA1-8F7A-68895670946A}" name="Assignee" dataDxfId="289"/>
-    <tableColumn id="26" xr3:uid="{8B283F34-2401-433E-BF9E-46632B6408A9}" name="Estimated effort" dataDxfId="288"/>
-    <tableColumn id="5" xr3:uid="{DA3B2E9F-6814-447A-ABDD-B51650B1F538}" name="Planned effort" dataDxfId="287">
+    <tableColumn id="1" xr3:uid="{01209A68-7F85-4C28-AFB5-81C5B0EC7A37}" name="Epic" dataDxfId="216"/>
+    <tableColumn id="2" xr3:uid="{66517A9E-46E1-41DF-9F0B-17AB54123296}" name="Ações" dataDxfId="215"/>
+    <tableColumn id="16" xr3:uid="{92F7750A-D683-45B5-80BF-2568989D936C}" name="Status" dataDxfId="214"/>
+    <tableColumn id="3" xr3:uid="{67DDF4A4-1CB4-4009-BCDB-046B5F84434E}" name="Due Date" dataDxfId="213"/>
+    <tableColumn id="4" xr3:uid="{CA9093F9-48BC-4FA1-8F7A-68895670946A}" name="Assignee" dataDxfId="212"/>
+    <tableColumn id="26" xr3:uid="{8B283F34-2401-433E-BF9E-46632B6408A9}" name="Estimated effort" dataDxfId="211"/>
+    <tableColumn id="5" xr3:uid="{DA3B2E9F-6814-447A-ABDD-B51650B1F538}" name="Planned effort" dataDxfId="210">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{917CBACF-F867-4934-9025-B36CB10603F2}" name="jul/24" dataDxfId="286"/>
-    <tableColumn id="9" xr3:uid="{FBFFE0A8-C6E4-409D-B23A-DF2E274C4084}" name="ago/24" dataDxfId="285"/>
-    <tableColumn id="10" xr3:uid="{284C8EFC-524F-4249-B0A3-46E07BCD0C6F}" name="set/24" dataDxfId="284"/>
-    <tableColumn id="11" xr3:uid="{B1B43394-E80B-493C-90C0-CCC233B09963}" name="out/24" dataDxfId="283"/>
-    <tableColumn id="12" xr3:uid="{297447F5-FC07-4D69-A994-F56BBE329C04}" name="nov/24" dataDxfId="282"/>
-    <tableColumn id="13" xr3:uid="{63D90C2A-07A2-428E-A98A-BC63F2B4DB88}" name="dez/24" dataDxfId="281"/>
-    <tableColumn id="14" xr3:uid="{0161802C-C4F0-4DC6-A5DF-0CBDAFE3EC56}" name="jan/25" dataDxfId="280"/>
-    <tableColumn id="15" xr3:uid="{4622BD16-94DE-42BA-AB00-AEDAEB6DAAB3}" name="fev/25" dataDxfId="279"/>
-    <tableColumn id="19" xr3:uid="{6E9E22F5-E9B1-428A-8E88-E9956E21ED68}" name="mar/25" dataDxfId="278"/>
-    <tableColumn id="21" xr3:uid="{C371C2C0-26B8-4188-9D83-B9F02BF26874}" name="abr/25" dataDxfId="277"/>
-    <tableColumn id="22" xr3:uid="{0279FDF5-E694-4716-8D32-683FA8E40DC7}" name="mai/25" dataDxfId="276"/>
-    <tableColumn id="20" xr3:uid="{01504503-6E36-42E2-9D08-552B1C4DA841}" name="jun/25" dataDxfId="275"/>
-    <tableColumn id="18" xr3:uid="{6981EBCE-7629-47D1-9EC5-76635D7EEC11}" name="jul/25" dataDxfId="274"/>
-    <tableColumn id="6" xr3:uid="{7CECE26F-F2E1-4D1C-BE7F-2F5C5C6C8949}" name="ago/25" dataDxfId="273"/>
-    <tableColumn id="7" xr3:uid="{AC3CED15-CFF9-4CE9-93BD-6AD7114C2285}" name="set/25" dataDxfId="272"/>
-    <tableColumn id="23" xr3:uid="{4421CF49-AB56-4301-BE99-45FCBA458FE9}" name="out/25" dataDxfId="271"/>
-    <tableColumn id="24" xr3:uid="{F1E3BB55-ED52-4ABB-A642-0180E60B91A1}" name="nov/25" dataDxfId="270"/>
-    <tableColumn id="25" xr3:uid="{C5C6F9DA-C654-4668-9412-C46C2E27CCB5}" name="dez/25" dataDxfId="269"/>
-    <tableColumn id="17" xr3:uid="{453C1F02-B3C0-420A-8706-84820C436FC0}" name="Nota" dataDxfId="268"/>
+    <tableColumn id="8" xr3:uid="{917CBACF-F867-4934-9025-B36CB10603F2}" name="jul/24" dataDxfId="209"/>
+    <tableColumn id="9" xr3:uid="{FBFFE0A8-C6E4-409D-B23A-DF2E274C4084}" name="ago/24" dataDxfId="208"/>
+    <tableColumn id="10" xr3:uid="{284C8EFC-524F-4249-B0A3-46E07BCD0C6F}" name="set/24" dataDxfId="207"/>
+    <tableColumn id="11" xr3:uid="{B1B43394-E80B-493C-90C0-CCC233B09963}" name="out/24" dataDxfId="206"/>
+    <tableColumn id="12" xr3:uid="{297447F5-FC07-4D69-A994-F56BBE329C04}" name="nov/24" dataDxfId="205"/>
+    <tableColumn id="13" xr3:uid="{63D90C2A-07A2-428E-A98A-BC63F2B4DB88}" name="dez/24" dataDxfId="204"/>
+    <tableColumn id="14" xr3:uid="{0161802C-C4F0-4DC6-A5DF-0CBDAFE3EC56}" name="jan/25" dataDxfId="203"/>
+    <tableColumn id="15" xr3:uid="{4622BD16-94DE-42BA-AB00-AEDAEB6DAAB3}" name="fev/25" dataDxfId="202"/>
+    <tableColumn id="19" xr3:uid="{6E9E22F5-E9B1-428A-8E88-E9956E21ED68}" name="mar/25" dataDxfId="201"/>
+    <tableColumn id="21" xr3:uid="{C371C2C0-26B8-4188-9D83-B9F02BF26874}" name="abr/25" dataDxfId="200"/>
+    <tableColumn id="22" xr3:uid="{0279FDF5-E694-4716-8D32-683FA8E40DC7}" name="mai/25" dataDxfId="199"/>
+    <tableColumn id="20" xr3:uid="{01504503-6E36-42E2-9D08-552B1C4DA841}" name="jun/25" dataDxfId="198"/>
+    <tableColumn id="18" xr3:uid="{6981EBCE-7629-47D1-9EC5-76635D7EEC11}" name="jul/25" dataDxfId="197"/>
+    <tableColumn id="6" xr3:uid="{7CECE26F-F2E1-4D1C-BE7F-2F5C5C6C8949}" name="ago/25" dataDxfId="196"/>
+    <tableColumn id="7" xr3:uid="{AC3CED15-CFF9-4CE9-93BD-6AD7114C2285}" name="set/25" dataDxfId="195"/>
+    <tableColumn id="23" xr3:uid="{4421CF49-AB56-4301-BE99-45FCBA458FE9}" name="out/25" dataDxfId="194"/>
+    <tableColumn id="24" xr3:uid="{F1E3BB55-ED52-4ABB-A642-0180E60B91A1}" name="nov/25" dataDxfId="193"/>
+    <tableColumn id="25" xr3:uid="{C5C6F9DA-C654-4668-9412-C46C2E27CCB5}" name="dez/25" dataDxfId="192"/>
+    <tableColumn id="17" xr3:uid="{453C1F02-B3C0-420A-8706-84820C436FC0}" name="Nota" dataDxfId="191"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A94C4A-C1A4-4112-856E-92FC8D7969DB}" name="Tabela145672" displayName="Tabela145672" ref="A1:Z23" totalsRowShown="0" headerRowDxfId="267" dataDxfId="266">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3A94C4A-C1A4-4112-856E-92FC8D7969DB}" name="Tabela145672" displayName="Tabela145672" ref="A1:Z23" totalsRowShown="0" headerRowDxfId="190" dataDxfId="189">
   <autoFilter ref="A1:Z23" xr:uid="{60C5897C-4C10-4DE1-B6BC-B05ADF30BE1F}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{D0BFE29A-C08D-4432-A0D1-F5BE5FA9F7C1}" name="Epic" dataDxfId="265"/>
-    <tableColumn id="2" xr3:uid="{8C671275-798D-4FAE-B5BD-30E3E1A48122}" name="Ações" dataDxfId="264"/>
-    <tableColumn id="16" xr3:uid="{87C1349B-8437-416B-A33A-8FC6819705F2}" name="Status" dataDxfId="263"/>
-    <tableColumn id="3" xr3:uid="{DD7467F0-B52A-4287-98BB-B87528290064}" name="Due Date" dataDxfId="262"/>
-    <tableColumn id="4" xr3:uid="{F324EBCD-A36A-4F07-A779-792658877228}" name="Assignee" dataDxfId="261"/>
-    <tableColumn id="26" xr3:uid="{8DE983D0-027C-4450-A1DC-946435E1A13E}" name="Estimated effort" dataDxfId="260"/>
-    <tableColumn id="5" xr3:uid="{12DD7B93-535D-43AB-9973-CAE08773A991}" name="Planned effort" dataDxfId="259">
+    <tableColumn id="1" xr3:uid="{D0BFE29A-C08D-4432-A0D1-F5BE5FA9F7C1}" name="Epic" dataDxfId="188"/>
+    <tableColumn id="2" xr3:uid="{8C671275-798D-4FAE-B5BD-30E3E1A48122}" name="Ações" dataDxfId="187"/>
+    <tableColumn id="16" xr3:uid="{87C1349B-8437-416B-A33A-8FC6819705F2}" name="Status" dataDxfId="186"/>
+    <tableColumn id="3" xr3:uid="{DD7467F0-B52A-4287-98BB-B87528290064}" name="Due Date" dataDxfId="185"/>
+    <tableColumn id="4" xr3:uid="{F324EBCD-A36A-4F07-A779-792658877228}" name="Assignee" dataDxfId="184"/>
+    <tableColumn id="26" xr3:uid="{8DE983D0-027C-4450-A1DC-946435E1A13E}" name="Estimated effort" dataDxfId="183"/>
+    <tableColumn id="5" xr3:uid="{12DD7B93-535D-43AB-9973-CAE08773A991}" name="Planned effort" dataDxfId="182">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{02ADA71E-139A-44BD-9DBE-52E2397E9F99}" name="jul/24" dataDxfId="258"/>
-    <tableColumn id="9" xr3:uid="{66CDD522-0887-4D47-B9AB-D9120C8F8652}" name="ago/24" dataDxfId="257"/>
-    <tableColumn id="10" xr3:uid="{215A1C1D-4C92-4B36-A568-FC96B9E55386}" name="set/24" dataDxfId="256"/>
-    <tableColumn id="11" xr3:uid="{CBBF2992-344C-4265-8B19-EFC408719519}" name="out/24" dataDxfId="255"/>
-    <tableColumn id="12" xr3:uid="{48354FF2-5862-4C42-8872-067CDAF119B8}" name="nov/24" dataDxfId="254"/>
-    <tableColumn id="13" xr3:uid="{86BA7996-57D5-4CBC-89F0-179CE30E92B5}" name="dez/24" dataDxfId="253"/>
-    <tableColumn id="14" xr3:uid="{DD0DE629-DE11-4498-AFAA-0A90A34ECD15}" name="jan/25" dataDxfId="252"/>
-    <tableColumn id="15" xr3:uid="{61B217CD-E5B3-4179-9B67-CD5D83039A82}" name="fev/25" dataDxfId="251"/>
-    <tableColumn id="19" xr3:uid="{12C2F4A2-445E-45C3-9AB8-532E78409774}" name="mar/25" dataDxfId="250"/>
-    <tableColumn id="21" xr3:uid="{6A279519-CE46-4260-A34A-5B0F223C1AEF}" name="abr/25" dataDxfId="249"/>
-    <tableColumn id="22" xr3:uid="{7D22944D-1A3C-417D-AABF-C1E11C55463F}" name="mai/25" dataDxfId="248"/>
-    <tableColumn id="20" xr3:uid="{53AAF552-291E-493E-8085-12CAB74C1603}" name="jun/25" dataDxfId="247"/>
-    <tableColumn id="18" xr3:uid="{EE160A5B-3CE9-4ADF-858B-5BC8EB110BB8}" name="jul/25" dataDxfId="246"/>
-    <tableColumn id="6" xr3:uid="{62845F62-5ED9-470F-9FDE-79786F4314EE}" name="ago/25" dataDxfId="245"/>
-    <tableColumn id="7" xr3:uid="{D3F062AF-DFE8-4C18-8946-1A4BF9A0BCE8}" name="set/25" dataDxfId="244"/>
-    <tableColumn id="23" xr3:uid="{B1C5C80E-32AB-4A68-96EA-AF37C4ECD963}" name="out/25" dataDxfId="243"/>
-    <tableColumn id="24" xr3:uid="{E7C40D8D-53C9-4E93-8BEC-EBE80515EFA0}" name="nov/25" dataDxfId="242"/>
-    <tableColumn id="25" xr3:uid="{05ACD4D3-D719-4C00-9722-A69C1E8DA9A7}" name="dez/25" dataDxfId="241"/>
-    <tableColumn id="17" xr3:uid="{7A812258-3D63-4F32-B797-9EFE1CF6C9E0}" name="Nota" dataDxfId="240"/>
+    <tableColumn id="8" xr3:uid="{02ADA71E-139A-44BD-9DBE-52E2397E9F99}" name="jul/24" dataDxfId="181"/>
+    <tableColumn id="9" xr3:uid="{66CDD522-0887-4D47-B9AB-D9120C8F8652}" name="ago/24" dataDxfId="180"/>
+    <tableColumn id="10" xr3:uid="{215A1C1D-4C92-4B36-A568-FC96B9E55386}" name="set/24" dataDxfId="179"/>
+    <tableColumn id="11" xr3:uid="{CBBF2992-344C-4265-8B19-EFC408719519}" name="out/24" dataDxfId="178"/>
+    <tableColumn id="12" xr3:uid="{48354FF2-5862-4C42-8872-067CDAF119B8}" name="nov/24" dataDxfId="177"/>
+    <tableColumn id="13" xr3:uid="{86BA7996-57D5-4CBC-89F0-179CE30E92B5}" name="dez/24" dataDxfId="176"/>
+    <tableColumn id="14" xr3:uid="{DD0DE629-DE11-4498-AFAA-0A90A34ECD15}" name="jan/25" dataDxfId="175"/>
+    <tableColumn id="15" xr3:uid="{61B217CD-E5B3-4179-9B67-CD5D83039A82}" name="fev/25" dataDxfId="174"/>
+    <tableColumn id="19" xr3:uid="{12C2F4A2-445E-45C3-9AB8-532E78409774}" name="mar/25" dataDxfId="173"/>
+    <tableColumn id="21" xr3:uid="{6A279519-CE46-4260-A34A-5B0F223C1AEF}" name="abr/25" dataDxfId="172"/>
+    <tableColumn id="22" xr3:uid="{7D22944D-1A3C-417D-AABF-C1E11C55463F}" name="mai/25" dataDxfId="171"/>
+    <tableColumn id="20" xr3:uid="{53AAF552-291E-493E-8085-12CAB74C1603}" name="jun/25" dataDxfId="170"/>
+    <tableColumn id="18" xr3:uid="{EE160A5B-3CE9-4ADF-858B-5BC8EB110BB8}" name="jul/25" dataDxfId="169"/>
+    <tableColumn id="6" xr3:uid="{62845F62-5ED9-470F-9FDE-79786F4314EE}" name="ago/25" dataDxfId="168"/>
+    <tableColumn id="7" xr3:uid="{D3F062AF-DFE8-4C18-8946-1A4BF9A0BCE8}" name="set/25" dataDxfId="167"/>
+    <tableColumn id="23" xr3:uid="{B1C5C80E-32AB-4A68-96EA-AF37C4ECD963}" name="out/25" dataDxfId="166"/>
+    <tableColumn id="24" xr3:uid="{E7C40D8D-53C9-4E93-8BEC-EBE80515EFA0}" name="nov/25" dataDxfId="165"/>
+    <tableColumn id="25" xr3:uid="{05ACD4D3-D719-4C00-9722-A69C1E8DA9A7}" name="dez/25" dataDxfId="164"/>
+    <tableColumn id="17" xr3:uid="{7A812258-3D63-4F32-B797-9EFE1CF6C9E0}" name="Nota" dataDxfId="163"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CE7B39CA-9CEA-443A-A1B1-DF25F95E1766}" name="Tabela14567" displayName="Tabela14567" ref="A1:Z23" totalsRowShown="0" headerRowDxfId="239" dataDxfId="238">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CE7B39CA-9CEA-443A-A1B1-DF25F95E1766}" name="Tabela14567" displayName="Tabela14567" ref="A1:Z23" totalsRowShown="0" headerRowDxfId="162" dataDxfId="161">
   <autoFilter ref="A1:Z23" xr:uid="{60C5897C-4C10-4DE1-B6BC-B05ADF30BE1F}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{EE289A6C-5700-4272-9B32-66B5A70B31CB}" name="Epic" dataDxfId="237"/>
-    <tableColumn id="2" xr3:uid="{EC48C96C-B497-45F2-BF0A-9811794FDB1D}" name="Ações" dataDxfId="236"/>
-    <tableColumn id="16" xr3:uid="{BDD02027-9F42-4199-8375-236F74D7FDCD}" name="Status" dataDxfId="235"/>
-    <tableColumn id="3" xr3:uid="{F770666B-765B-41DC-A5CE-B6DF39D0880D}" name="Due Date" dataDxfId="234"/>
-    <tableColumn id="4" xr3:uid="{5940F227-9D6D-4C88-BE63-5D2D86568E14}" name="Assignee" dataDxfId="233"/>
-    <tableColumn id="26" xr3:uid="{7BC9F0AA-006F-42E4-A33B-D4009B68631E}" name="Estimated effort" dataDxfId="232"/>
-    <tableColumn id="5" xr3:uid="{4508400F-4340-4A7A-8115-85F48DCC6A1F}" name="Planned effort" dataDxfId="231">
+    <tableColumn id="1" xr3:uid="{EE289A6C-5700-4272-9B32-66B5A70B31CB}" name="Epic" dataDxfId="160"/>
+    <tableColumn id="2" xr3:uid="{EC48C96C-B497-45F2-BF0A-9811794FDB1D}" name="Ações" dataDxfId="159"/>
+    <tableColumn id="16" xr3:uid="{BDD02027-9F42-4199-8375-236F74D7FDCD}" name="Status" dataDxfId="158"/>
+    <tableColumn id="3" xr3:uid="{F770666B-765B-41DC-A5CE-B6DF39D0880D}" name="Due Date" dataDxfId="157"/>
+    <tableColumn id="4" xr3:uid="{5940F227-9D6D-4C88-BE63-5D2D86568E14}" name="Assignee" dataDxfId="156"/>
+    <tableColumn id="26" xr3:uid="{7BC9F0AA-006F-42E4-A33B-D4009B68631E}" name="Estimated effort" dataDxfId="155"/>
+    <tableColumn id="5" xr3:uid="{4508400F-4340-4A7A-8115-85F48DCC6A1F}" name="Planned effort" dataDxfId="154">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7EAC2713-0D8D-4F34-BB97-2E13833E1F97}" name="jul/24" dataDxfId="230"/>
-    <tableColumn id="9" xr3:uid="{D91CD170-23D2-4F07-A973-2711FED7E661}" name="ago/24" dataDxfId="229"/>
-    <tableColumn id="10" xr3:uid="{F554D11D-299C-4300-BF37-0DFE32B55E1C}" name="set/24" dataDxfId="228"/>
-    <tableColumn id="11" xr3:uid="{628228E9-61C6-4983-83EE-A19EA3F02BE4}" name="out/24" dataDxfId="227"/>
-    <tableColumn id="12" xr3:uid="{CAC0DDF3-5B4D-4943-81CB-ABC1F647F25B}" name="nov/24" dataDxfId="226"/>
-    <tableColumn id="13" xr3:uid="{5EAED47A-4FF0-4D6D-8534-DA5876F11ED0}" name="dez/24" dataDxfId="225"/>
-    <tableColumn id="14" xr3:uid="{84BC7C3E-66D3-434E-A1B1-A9A5E9F04C22}" name="jan/25" dataDxfId="224"/>
-    <tableColumn id="15" xr3:uid="{9DC7E363-E618-46CA-8851-4EA5DA2A6C04}" name="fev/25" dataDxfId="223"/>
-    <tableColumn id="19" xr3:uid="{C8B10481-AD95-45F8-985D-4D981DB0BDC3}" name="mar/25" dataDxfId="222"/>
-    <tableColumn id="21" xr3:uid="{CF87C928-2C06-476C-9082-F3D54DA57F4C}" name="abr/25" dataDxfId="221"/>
-    <tableColumn id="22" xr3:uid="{B675A93E-7C58-4534-BEBC-6878075475C3}" name="mai/25" dataDxfId="220"/>
-    <tableColumn id="20" xr3:uid="{63D8B4DF-D8ED-4826-BEEB-D47DB0107DAA}" name="jun/25" dataDxfId="219"/>
-    <tableColumn id="18" xr3:uid="{CF776872-834C-4BB2-B773-F21A743F80F1}" name="jul/25" dataDxfId="218"/>
-    <tableColumn id="6" xr3:uid="{631FADD6-5D6F-4227-8B64-8DF1CD5E37C2}" name="ago/25" dataDxfId="217"/>
-    <tableColumn id="7" xr3:uid="{75C45859-3E26-4B6E-9A75-C8428CCA97B8}" name="set/25" dataDxfId="216"/>
-    <tableColumn id="23" xr3:uid="{8A7800BA-3CD6-4A83-BEBF-5AE3FF1D781B}" name="out/25" dataDxfId="215"/>
-    <tableColumn id="24" xr3:uid="{64C38EBA-0572-4482-A323-078F1D86FEFC}" name="nov/25" dataDxfId="214"/>
-    <tableColumn id="17" xr3:uid="{B19F5706-C1C9-4677-A883-C6B40ECCF96B}" name="dez/25" dataDxfId="213"/>
-    <tableColumn id="25" xr3:uid="{52ABDA5C-8FA8-4D59-BCBD-6C0B42E314C2}" name="Nota" dataDxfId="212"/>
+    <tableColumn id="8" xr3:uid="{7EAC2713-0D8D-4F34-BB97-2E13833E1F97}" name="jul/24" dataDxfId="153"/>
+    <tableColumn id="9" xr3:uid="{D91CD170-23D2-4F07-A973-2711FED7E661}" name="ago/24" dataDxfId="152"/>
+    <tableColumn id="10" xr3:uid="{F554D11D-299C-4300-BF37-0DFE32B55E1C}" name="set/24" dataDxfId="151"/>
+    <tableColumn id="11" xr3:uid="{628228E9-61C6-4983-83EE-A19EA3F02BE4}" name="out/24" dataDxfId="150"/>
+    <tableColumn id="12" xr3:uid="{CAC0DDF3-5B4D-4943-81CB-ABC1F647F25B}" name="nov/24" dataDxfId="149"/>
+    <tableColumn id="13" xr3:uid="{5EAED47A-4FF0-4D6D-8534-DA5876F11ED0}" name="dez/24" dataDxfId="148"/>
+    <tableColumn id="14" xr3:uid="{84BC7C3E-66D3-434E-A1B1-A9A5E9F04C22}" name="jan/25" dataDxfId="147"/>
+    <tableColumn id="15" xr3:uid="{9DC7E363-E618-46CA-8851-4EA5DA2A6C04}" name="fev/25" dataDxfId="146"/>
+    <tableColumn id="19" xr3:uid="{C8B10481-AD95-45F8-985D-4D981DB0BDC3}" name="mar/25" dataDxfId="145"/>
+    <tableColumn id="21" xr3:uid="{CF87C928-2C06-476C-9082-F3D54DA57F4C}" name="abr/25" dataDxfId="144"/>
+    <tableColumn id="22" xr3:uid="{B675A93E-7C58-4534-BEBC-6878075475C3}" name="mai/25" dataDxfId="143"/>
+    <tableColumn id="20" xr3:uid="{63D8B4DF-D8ED-4826-BEEB-D47DB0107DAA}" name="jun/25" dataDxfId="142"/>
+    <tableColumn id="18" xr3:uid="{CF776872-834C-4BB2-B773-F21A743F80F1}" name="jul/25" dataDxfId="141"/>
+    <tableColumn id="6" xr3:uid="{631FADD6-5D6F-4227-8B64-8DF1CD5E37C2}" name="ago/25" dataDxfId="140"/>
+    <tableColumn id="7" xr3:uid="{75C45859-3E26-4B6E-9A75-C8428CCA97B8}" name="set/25" dataDxfId="139"/>
+    <tableColumn id="23" xr3:uid="{8A7800BA-3CD6-4A83-BEBF-5AE3FF1D781B}" name="out/25" dataDxfId="138"/>
+    <tableColumn id="24" xr3:uid="{64C38EBA-0572-4482-A323-078F1D86FEFC}" name="nov/25" dataDxfId="137"/>
+    <tableColumn id="17" xr3:uid="{B19F5706-C1C9-4677-A883-C6B40ECCF96B}" name="dez/25" dataDxfId="136"/>
+    <tableColumn id="25" xr3:uid="{52ABDA5C-8FA8-4D59-BCBD-6C0B42E314C2}" name="Nota" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73520871-8519-4F69-99C7-ADB749126326}" name="Tabela1456724" displayName="Tabela1456724" ref="A1:Z28" totalsRowShown="0" headerRowDxfId="211" dataDxfId="210">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73520871-8519-4F69-99C7-ADB749126326}" name="Tabela1456724" displayName="Tabela1456724" ref="A1:Z28" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
   <autoFilter ref="A1:Z28" xr:uid="{60C5897C-4C10-4DE1-B6BC-B05ADF30BE1F}">
     <filterColumn colId="2">
       <filters blank="1">
@@ -2960,41 +2435,41 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{F7B1E8EA-C0EC-458C-BE1D-C9AAC078AC40}" name="Epic" dataDxfId="209"/>
-    <tableColumn id="2" xr3:uid="{AE5B099A-8CF9-4A5A-98FD-30B800510534}" name="Ações" dataDxfId="208"/>
-    <tableColumn id="16" xr3:uid="{2D90475A-D5BC-4CB2-858A-AAEA8DBCD03F}" name="Status" dataDxfId="207"/>
-    <tableColumn id="3" xr3:uid="{62D10A36-6221-4217-9B01-29C8D1055992}" name="Due Date" dataDxfId="206"/>
-    <tableColumn id="4" xr3:uid="{1A6879A9-9799-4837-9BD6-F28346B95C2A}" name="Assignee" dataDxfId="205"/>
-    <tableColumn id="26" xr3:uid="{95502097-81FF-4227-B76B-75D5B47EDAB8}" name="Estimated effort" dataDxfId="204"/>
-    <tableColumn id="5" xr3:uid="{17C94D3B-8E75-4800-A1F4-1F1988CAAB97}" name="Planned effort" dataDxfId="203">
+    <tableColumn id="1" xr3:uid="{F7B1E8EA-C0EC-458C-BE1D-C9AAC078AC40}" name="Epic" dataDxfId="132"/>
+    <tableColumn id="2" xr3:uid="{AE5B099A-8CF9-4A5A-98FD-30B800510534}" name="Ações" dataDxfId="131"/>
+    <tableColumn id="16" xr3:uid="{2D90475A-D5BC-4CB2-858A-AAEA8DBCD03F}" name="Status" dataDxfId="130"/>
+    <tableColumn id="3" xr3:uid="{62D10A36-6221-4217-9B01-29C8D1055992}" name="Due Date" dataDxfId="129"/>
+    <tableColumn id="4" xr3:uid="{1A6879A9-9799-4837-9BD6-F28346B95C2A}" name="Assignee" dataDxfId="128"/>
+    <tableColumn id="26" xr3:uid="{95502097-81FF-4227-B76B-75D5B47EDAB8}" name="Estimated effort" dataDxfId="127"/>
+    <tableColumn id="5" xr3:uid="{17C94D3B-8E75-4800-A1F4-1F1988CAAB97}" name="Planned effort" dataDxfId="126">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{452C87B7-00A2-49F6-B03C-09B1516BF610}" name="jul/24" dataDxfId="202"/>
-    <tableColumn id="9" xr3:uid="{9D968673-E47A-4771-ACDB-1F92433F2F49}" name="ago/24" dataDxfId="201"/>
-    <tableColumn id="10" xr3:uid="{06622939-253A-4451-9DF1-AEBDBBA61691}" name="set/24" dataDxfId="200"/>
-    <tableColumn id="11" xr3:uid="{FD9CB1DD-EDF9-42FC-9707-AE7332F0860E}" name="out/24" dataDxfId="199"/>
-    <tableColumn id="12" xr3:uid="{C11EE033-846E-4BF8-B958-62468811794F}" name="nov/24" dataDxfId="198"/>
-    <tableColumn id="13" xr3:uid="{665BFD75-9AA2-4E96-ADDE-9AE9F9D127BD}" name="dez/24" dataDxfId="197"/>
-    <tableColumn id="14" xr3:uid="{518E6267-8E42-43E3-A70F-F9B5F74C3A5D}" name="jan/25" dataDxfId="196"/>
-    <tableColumn id="15" xr3:uid="{59E259D1-C4C8-4310-AA50-AE6BDDAD209B}" name="fev/25" dataDxfId="195"/>
-    <tableColumn id="19" xr3:uid="{9A7ADD22-96F1-4C43-A976-D9612862FA01}" name="mar/25" dataDxfId="194"/>
-    <tableColumn id="21" xr3:uid="{51B1E82E-5665-407F-8866-78296B84F2BC}" name="abr/25" dataDxfId="193"/>
-    <tableColumn id="22" xr3:uid="{6C7FFD66-47DC-4EB5-AB00-BCD0B62EC755}" name="mai/25" dataDxfId="192"/>
-    <tableColumn id="20" xr3:uid="{FE0847CB-FF6C-474A-B100-D4A8BF538F92}" name="jun/25" dataDxfId="191"/>
-    <tableColumn id="18" xr3:uid="{E352B795-3F0A-4277-B11A-F584AF2B6AD2}" name="jul/25" dataDxfId="190"/>
-    <tableColumn id="6" xr3:uid="{A09C9E60-8686-4233-A1BC-CFC5A282979E}" name="ago/25" dataDxfId="189"/>
-    <tableColumn id="7" xr3:uid="{F2213C78-02EB-4765-B1A1-2C0398B8FCC0}" name="set/25" dataDxfId="188"/>
-    <tableColumn id="23" xr3:uid="{242DEB15-224E-4660-9784-7BD0207173DD}" name="out/25" dataDxfId="187"/>
-    <tableColumn id="24" xr3:uid="{2F378A4B-5F7F-4B88-94E1-BE64D0451DDD}" name="nov/25" dataDxfId="186"/>
-    <tableColumn id="25" xr3:uid="{82B623CC-2A7F-472A-B629-207037C10DC9}" name="dez/25" dataDxfId="185"/>
-    <tableColumn id="17" xr3:uid="{9E9D8F62-32C3-4D66-A66D-846E7A302BD3}" name="Nota" dataDxfId="184"/>
+    <tableColumn id="8" xr3:uid="{452C87B7-00A2-49F6-B03C-09B1516BF610}" name="jul/24" dataDxfId="125"/>
+    <tableColumn id="9" xr3:uid="{9D968673-E47A-4771-ACDB-1F92433F2F49}" name="ago/24" dataDxfId="124"/>
+    <tableColumn id="10" xr3:uid="{06622939-253A-4451-9DF1-AEBDBBA61691}" name="set/24" dataDxfId="123"/>
+    <tableColumn id="11" xr3:uid="{FD9CB1DD-EDF9-42FC-9707-AE7332F0860E}" name="out/24" dataDxfId="122"/>
+    <tableColumn id="12" xr3:uid="{C11EE033-846E-4BF8-B958-62468811794F}" name="nov/24" dataDxfId="121"/>
+    <tableColumn id="13" xr3:uid="{665BFD75-9AA2-4E96-ADDE-9AE9F9D127BD}" name="dez/24" dataDxfId="120"/>
+    <tableColumn id="14" xr3:uid="{518E6267-8E42-43E3-A70F-F9B5F74C3A5D}" name="jan/25" dataDxfId="119"/>
+    <tableColumn id="15" xr3:uid="{59E259D1-C4C8-4310-AA50-AE6BDDAD209B}" name="fev/25" dataDxfId="118"/>
+    <tableColumn id="19" xr3:uid="{9A7ADD22-96F1-4C43-A976-D9612862FA01}" name="mar/25" dataDxfId="117"/>
+    <tableColumn id="21" xr3:uid="{51B1E82E-5665-407F-8866-78296B84F2BC}" name="abr/25" dataDxfId="116"/>
+    <tableColumn id="22" xr3:uid="{6C7FFD66-47DC-4EB5-AB00-BCD0B62EC755}" name="mai/25" dataDxfId="115"/>
+    <tableColumn id="20" xr3:uid="{FE0847CB-FF6C-474A-B100-D4A8BF538F92}" name="jun/25" dataDxfId="114"/>
+    <tableColumn id="18" xr3:uid="{E352B795-3F0A-4277-B11A-F584AF2B6AD2}" name="jul/25" dataDxfId="113"/>
+    <tableColumn id="6" xr3:uid="{A09C9E60-8686-4233-A1BC-CFC5A282979E}" name="ago/25" dataDxfId="112"/>
+    <tableColumn id="7" xr3:uid="{F2213C78-02EB-4765-B1A1-2C0398B8FCC0}" name="set/25" dataDxfId="111"/>
+    <tableColumn id="23" xr3:uid="{242DEB15-224E-4660-9784-7BD0207173DD}" name="out/25" dataDxfId="110"/>
+    <tableColumn id="24" xr3:uid="{2F378A4B-5F7F-4B88-94E1-BE64D0451DDD}" name="nov/25" dataDxfId="109"/>
+    <tableColumn id="25" xr3:uid="{82B623CC-2A7F-472A-B629-207037C10DC9}" name="dez/25" dataDxfId="108"/>
+    <tableColumn id="17" xr3:uid="{9E9D8F62-32C3-4D66-A66D-846E7A302BD3}" name="Nota" dataDxfId="107"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3292,7 +2767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6104E23D-49AE-4821-BB68-D70F1BB52886}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
@@ -3713,12 +3188,8 @@
       <c r="T7" s="11"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="32" t="e">
+      <c r="G8" s="6" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
@@ -3737,12 +3208,8 @@
       <c r="T8" s="5"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="32" t="e">
+      <c r="G9" s="6" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
@@ -4239,242 +3706,143 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A23:C23 P15:Q15 H13:O15 H16:Q19 A21:B21 H21:Q21 R13:T21 H22:T23">
-    <cfRule type="expression" dxfId="183" priority="177">
-      <formula>IF($A13="Esforço total atribuído",1)</formula>
+  <conditionalFormatting sqref="A7:A13">
+    <cfRule type="expression" dxfId="106" priority="1">
+      <formula>IF($A7="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="178">
-      <formula>IF($A13="Disponibilidade restante",1)</formula>
+    <cfRule type="expression" dxfId="105" priority="2">
+      <formula>IF($A7="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="179">
-      <formula>IF($A13="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="104" priority="3">
+      <formula>IF($A7="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="180">
+    <cfRule type="expression" dxfId="103" priority="4">
+      <formula>IF($B7=1,1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:B30">
+    <cfRule type="expression" dxfId="102" priority="36">
+      <formula>IF(#REF!=1,1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="35">
+      <formula>IF($A24="Disponibil.total",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="34">
+      <formula>IF($A24="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="33">
+      <formula>IF($A24="Esforço total atribuído",1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="expression" dxfId="98" priority="5">
+      <formula>IF($A18="Esforço total atribuído",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="6">
+      <formula>IF($A18="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="7">
+      <formula>IF($A18="Disponibil.total",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="8">
+      <formula>IF($B18=1,1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:N20">
+    <cfRule type="expression" dxfId="94" priority="143">
+      <formula>IF($A20="Disponibil.total",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="142">
+      <formula>IF($A20="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="141">
+      <formula>IF($A20="Esforço total atribuído",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="144">
       <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H13:O15 R13:T21 H16:Q19 A21:B21 H21:Q21 H22:T23 A23:C23">
+    <cfRule type="expression" dxfId="90" priority="180">
+      <formula>IF(#REF!=1,1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="178">
+      <formula>IF($A13="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="179">
+      <formula>IF($A13="Disponibil.total",1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:T23 H16:Q19 H13:O15 R13:T21 A21:B21 H21:Q21 A23:C23">
+    <cfRule type="expression" dxfId="87" priority="177">
+      <formula>IF($A13="Esforço total atribuído",1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:T30">
+    <cfRule type="expression" dxfId="86" priority="20">
+      <formula>IF($B24=1,1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="19">
+      <formula>IF($A24="Disponibil.total",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="18">
+      <formula>IF($A24="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="17">
+      <formula>IF($A24="Esforço total atribuído",1)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O20:Q20">
-    <cfRule type="expression" dxfId="179" priority="145">
+    <cfRule type="expression" dxfId="82" priority="147">
+      <formula>IF($A20="Disponibil.total",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="146">
+      <formula>IF($A20="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="145">
       <formula>IF($A20="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="146">
-      <formula>IF($A20="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="177" priority="147">
-      <formula>IF($A20="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="176" priority="148">
-      <formula>IF(#REF!=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20:N20">
-    <cfRule type="expression" dxfId="175" priority="141">
-      <formula>IF($A20="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="174" priority="142">
-      <formula>IF($A20="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="173" priority="143">
-      <formula>IF($A20="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="172" priority="144">
+    <cfRule type="expression" dxfId="79" priority="148">
       <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23:T23">
-    <cfRule type="expression" dxfId="171" priority="137">
+    <cfRule type="expression" dxfId="78" priority="139">
+      <formula>IF($A23="Disponibil.total",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="138">
+      <formula>IF($A23="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="137">
       <formula>IF($A23="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="138">
-      <formula>IF($A23="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="169" priority="139">
-      <formula>IF($A23="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="168" priority="140">
+    <cfRule type="expression" dxfId="75" priority="140">
       <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P14:Q14">
-    <cfRule type="expression" dxfId="167" priority="73">
-      <formula>IF($A14="Esforço total atribuído",1)</formula>
+  <conditionalFormatting sqref="P13:Q19">
+    <cfRule type="expression" dxfId="74" priority="62">
+      <formula>IF($A13="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="74">
-      <formula>IF($A14="Disponibilidade restante",1)</formula>
+    <cfRule type="expression" dxfId="73" priority="61">
+      <formula>IF($A13="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="75">
-      <formula>IF($A14="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="72" priority="63">
+      <formula>IF($A13="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="76">
+    <cfRule type="expression" dxfId="71" priority="44">
       <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P13:Q13">
-    <cfRule type="expression" dxfId="163" priority="69">
-      <formula>IF($A13="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="162" priority="70">
-      <formula>IF($A13="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="161" priority="71">
-      <formula>IF($A13="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="160" priority="72">
-      <formula>IF(#REF!=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P16:Q19">
-    <cfRule type="expression" dxfId="159" priority="61">
-      <formula>IF($A16="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="158" priority="62">
-      <formula>IF($A16="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="157" priority="63">
-      <formula>IF($A16="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="156" priority="64">
-      <formula>IF(#REF!=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P18:Q18">
-    <cfRule type="expression" dxfId="155" priority="57">
-      <formula>IF($A18="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="58">
+  <conditionalFormatting sqref="P18:Q19">
+    <cfRule type="expression" dxfId="70" priority="42">
       <formula>IF($A18="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="59">
+    <cfRule type="expression" dxfId="69" priority="43">
       <formula>IF($A18="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="60">
-      <formula>IF(#REF!=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P19:Q19">
-    <cfRule type="expression" dxfId="151" priority="41">
-      <formula>IF($A19="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="150" priority="42">
-      <formula>IF($A19="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="149" priority="43">
-      <formula>IF($A19="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="148" priority="44">
-      <formula>IF(#REF!=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24:B30">
-    <cfRule type="expression" dxfId="147" priority="33">
-      <formula>IF($A24="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="146" priority="34">
-      <formula>IF($A24="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="145" priority="35">
-      <formula>IF($A24="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="144" priority="36">
-      <formula>IF(#REF!=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24:J30">
-    <cfRule type="expression" dxfId="143" priority="29">
-      <formula>IF($A24="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="142" priority="30">
-      <formula>IF($A24="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="141" priority="31">
-      <formula>IF($A24="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="32">
-      <formula>IF($B24=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K24:M30">
-    <cfRule type="expression" dxfId="139" priority="25">
-      <formula>IF($A24="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="138" priority="26">
-      <formula>IF($A24="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="137" priority="27">
-      <formula>IF($A24="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="28">
-      <formula>IF($B24=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N24:P30">
-    <cfRule type="expression" dxfId="135" priority="21">
-      <formula>IF($A24="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="22">
-      <formula>IF($A24="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="133" priority="23">
-      <formula>IF($A24="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="132" priority="24">
-      <formula>IF($B24=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q24:T30">
-    <cfRule type="expression" dxfId="131" priority="17">
-      <formula>IF($A24="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="18">
-      <formula>IF($A24="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="129" priority="19">
-      <formula>IF($A24="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="128" priority="20">
-      <formula>IF($B24=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="expression" dxfId="127" priority="9">
-      <formula>IF($A13="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="10">
-      <formula>IF($A13="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="11">
-      <formula>IF($A13="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="124" priority="12">
-      <formula>IF($B13=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="123" priority="5">
+    <cfRule type="expression" dxfId="68" priority="41">
       <formula>IF($A18="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="122" priority="6">
-      <formula>IF($A18="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="121" priority="7">
-      <formula>IF($A18="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="120" priority="8">
-      <formula>IF($B18=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7:A12">
-    <cfRule type="expression" dxfId="119" priority="1">
-      <formula>IF($A7="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="2">
-      <formula>IF($A7="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="3">
-      <formula>IF($A7="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="4">
-      <formula>IF($B7=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4489,9 +3857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6CD8726-B30B-4400-9738-90F4E3A3D657}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4501,7 +3869,7 @@
     <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
@@ -6145,73 +5513,59 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A13:A15 A20:A31">
-    <cfRule type="expression" dxfId="115" priority="21">
+  <conditionalFormatting sqref="A13:A16">
+    <cfRule type="expression" dxfId="67" priority="9">
       <formula>IF($A13="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="22">
+    <cfRule type="expression" dxfId="66" priority="10">
       <formula>IF($A13="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="23">
+    <cfRule type="expression" dxfId="65" priority="11">
       <formula>IF($A13="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="24">
+    <cfRule type="expression" dxfId="64" priority="12">
       <formula>IF($B13=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="111" priority="13">
-      <formula>IF($A32="Esforço total atribuído",1)</formula>
+  <conditionalFormatting sqref="A20:A32">
+    <cfRule type="expression" dxfId="63" priority="13">
+      <formula>IF($A20="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="14">
-      <formula>IF($A32="Disponibilidade restante",1)</formula>
+    <cfRule type="expression" dxfId="62" priority="14">
+      <formula>IF($A20="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="15">
-      <formula>IF($A32="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="61" priority="15">
+      <formula>IF($A20="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="16">
-      <formula>IF($B32=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16">
-    <cfRule type="expression" dxfId="107" priority="9">
-      <formula>IF($A16="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="10">
-      <formula>IF($A16="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="11">
-      <formula>IF($A16="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="12">
-      <formula>IF($B16=1,1)</formula>
+    <cfRule type="expression" dxfId="60" priority="16">
+      <formula>IF($B20=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:Q3">
-    <cfRule type="expression" dxfId="103" priority="5">
+    <cfRule type="expression" dxfId="59" priority="5">
       <formula>IF($A3="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="6">
+    <cfRule type="expression" dxfId="58" priority="6">
       <formula>IF($A3="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="7">
+    <cfRule type="expression" dxfId="57" priority="7">
       <formula>IF($A3="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="8">
+    <cfRule type="expression" dxfId="56" priority="8">
       <formula>IF($B3=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:Y3">
-    <cfRule type="expression" dxfId="99" priority="1">
+    <cfRule type="expression" dxfId="55" priority="1">
       <formula>IF($A3="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="2">
+    <cfRule type="expression" dxfId="54" priority="2">
       <formula>IF($A3="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="3">
+    <cfRule type="expression" dxfId="53" priority="3">
       <formula>IF($A3="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="4">
+    <cfRule type="expression" dxfId="52" priority="4">
       <formula>IF($B3=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7853,115 +7207,73 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A23 A11:A14">
-    <cfRule type="expression" dxfId="95" priority="41">
+  <conditionalFormatting sqref="A11:A15">
+    <cfRule type="expression" dxfId="51" priority="25">
       <formula>IF($A11="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="42">
+    <cfRule type="expression" dxfId="50" priority="26">
       <formula>IF($A11="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="43">
+    <cfRule type="expression" dxfId="49" priority="27">
       <formula>IF($A11="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="44">
+    <cfRule type="expression" dxfId="48" priority="28">
       <formula>IF($B11=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="91" priority="25">
-      <formula>IF($A15="Esforço total atribuído",1)</formula>
+  <conditionalFormatting sqref="A17:A19">
+    <cfRule type="expression" dxfId="47" priority="9">
+      <formula>IF($A17="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="26">
-      <formula>IF($A15="Disponibilidade restante",1)</formula>
+    <cfRule type="expression" dxfId="46" priority="10">
+      <formula>IF($A17="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="27">
-      <formula>IF($A15="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="45" priority="11">
+      <formula>IF($A17="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="28">
-      <formula>IF($B15=1,1)</formula>
+    <cfRule type="expression" dxfId="44" priority="12">
+      <formula>IF($B17=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="87" priority="21">
+  <conditionalFormatting sqref="A22:A23">
+    <cfRule type="expression" dxfId="43" priority="21">
       <formula>IF($A22="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>IF($A22="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="23">
+    <cfRule type="expression" dxfId="41" priority="23">
       <formula>IF($A22="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="24">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>IF($B22=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="83" priority="17">
-      <formula>IF($A17="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="18">
-      <formula>IF($A17="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="19">
-      <formula>IF($A17="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="20">
-      <formula>IF($B17=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="79" priority="13">
-      <formula>IF($A18="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="14">
-      <formula>IF($A18="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="15">
-      <formula>IF($A18="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="16">
-      <formula>IF($B18=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="75" priority="9">
-      <formula>IF($A19="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="10">
-      <formula>IF($A19="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="11">
-      <formula>IF($A19="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="12">
-      <formula>IF($B19=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I3:Q3">
-    <cfRule type="expression" dxfId="71" priority="5">
+    <cfRule type="expression" dxfId="39" priority="5">
       <formula>IF($A3="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="6">
+    <cfRule type="expression" dxfId="38" priority="6">
       <formula>IF($A3="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="7">
+    <cfRule type="expression" dxfId="37" priority="7">
       <formula>IF($A3="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="8">
+    <cfRule type="expression" dxfId="36" priority="8">
       <formula>IF($B3=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:Y3">
-    <cfRule type="expression" dxfId="67" priority="1">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>IF($A3="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="2">
+    <cfRule type="expression" dxfId="34" priority="2">
       <formula>IF($A3="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>IF($A3="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="4">
+    <cfRule type="expression" dxfId="32" priority="4">
       <formula>IF($B3=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9389,73 +8701,59 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A23 A15:A16 A19:A21 A11:A13">
-    <cfRule type="expression" dxfId="63" priority="29">
+  <conditionalFormatting sqref="A11:A13 A23">
+    <cfRule type="expression" dxfId="31" priority="29">
       <formula>IF($A11="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="30">
+    <cfRule type="expression" dxfId="30" priority="30">
       <formula>IF($A11="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="31">
+    <cfRule type="expression" dxfId="29" priority="31">
       <formula>IF($A11="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="32">
+    <cfRule type="expression" dxfId="28" priority="32">
       <formula>IF($B11=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="59" priority="13">
-      <formula>IF($A17="Esforço total atribuído",1)</formula>
+  <conditionalFormatting sqref="A15:A21">
+    <cfRule type="expression" dxfId="27" priority="9">
+      <formula>IF($A15="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="14">
-      <formula>IF($A17="Disponibilidade restante",1)</formula>
+    <cfRule type="expression" dxfId="26" priority="10">
+      <formula>IF($A15="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="15">
-      <formula>IF($A17="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="25" priority="11">
+      <formula>IF($A15="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="16">
-      <formula>IF($B17=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="55" priority="9">
-      <formula>IF($A18="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="10">
-      <formula>IF($A18="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="11">
-      <formula>IF($A18="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="12">
-      <formula>IF($B18=1,1)</formula>
+    <cfRule type="expression" dxfId="24" priority="12">
+      <formula>IF($B15=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:Q3">
-    <cfRule type="expression" dxfId="51" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>IF($A3="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>IF($A3="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>IF($A3="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>IF($B3=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:Y3">
-    <cfRule type="expression" dxfId="47" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>IF($A3="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>IF($A3="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>IF($A3="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>IF($B3=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11518,130 +10816,32 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="expression" dxfId="43" priority="57">
-      <formula>IF($A27="Esforço total atribuído",1)</formula>
+  <conditionalFormatting sqref="A17:A20">
+    <cfRule type="expression" dxfId="15" priority="32">
+      <formula>IF($B17=1,1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="58">
-      <formula>IF($A27="Disponibilidade restante",1)</formula>
+    <cfRule type="expression" dxfId="14" priority="29">
+      <formula>IF($A17="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="59">
-      <formula>IF($A27="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="13" priority="30">
+      <formula>IF($A17="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="60">
-      <formula>IF($B27=1,1)</formula>
+    <cfRule type="expression" dxfId="12" priority="31">
+      <formula>IF($A17="Disponibil.total",1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="39" priority="53">
-      <formula>IF($A28="Esforço total atribuído",1)</formula>
+  <conditionalFormatting sqref="A22:A28">
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>IF($A22="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="54">
-      <formula>IF($A28="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="55">
-      <formula>IF($A28="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="56">
-      <formula>IF($B28=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="35" priority="49">
-      <formula>IF($A17="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="50">
-      <formula>IF($A17="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="51">
-      <formula>IF($A17="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="52">
-      <formula>IF($B17=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="31" priority="41">
-      <formula>IF($A18="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="42">
-      <formula>IF($A18="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="43">
-      <formula>IF($A18="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="44">
-      <formula>IF($B18=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:A20">
-    <cfRule type="expression" dxfId="27" priority="29">
-      <formula>IF($A19="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
-      <formula>IF($A19="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31">
-      <formula>IF($A19="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32">
-      <formula>IF($B19=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22 A26">
-    <cfRule type="expression" dxfId="23" priority="21">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>IF($A22="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="22">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>IF($A22="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="23">
-      <formula>IF($A22="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="24">
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>IF($B22=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="19" priority="17">
-      <formula>IF($A23="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
-      <formula>IF($A23="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="19">
-      <formula>IF($A23="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
-      <formula>IF($B23=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="15" priority="13">
-      <formula>IF($A24="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14">
-      <formula>IF($A24="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="15">
-      <formula>IF($A24="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>IF($B24=1,1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="11" priority="9">
-      <formula>IF($A25="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>IF($A25="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>IF($A25="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
-      <formula>IF($B25=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:Q3">
@@ -11659,17 +10859,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:Y3">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>IF($A3="Esforço total atribuído",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>IF($A3="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>IF($A3="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>IF($B3=1,1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF($A3="Esforço total atribuído",1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -11681,6 +10881,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010055299C8A5E56DF42BB3A496FAB31A3CA" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="f48546ee30a9c08b8c56cc99cae99613">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="886f8626-7949-4fe5-8403-a629ca357b95" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4da67acbd85d4947d1135fd4f9dd5422" ns2:_="">
     <xsd:import namespace="886f8626-7949-4fe5-8403-a629ca357b95"/>
@@ -11824,31 +11035,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64AD39B2-FED1-46F1-B570-2B06EBE1DD70}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E1C848C-A0C9-41E4-8BB1-646104CE90D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="886f8626-7949-4fe5-8403-a629ca357b95"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11870,9 +11060,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E1C848C-A0C9-41E4-8BB1-646104CE90D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64AD39B2-FED1-46F1-B570-2B06EBE1DD70}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="886f8626-7949-4fe5-8403-a629ca357b95"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add logica dinamica para possivel crescimento da planilha
</commit_message>
<xml_diff>
--- a/planilas-mari-weg/TIN Collaboration.xlsx
+++ b/planilas-mari-weg/TIN Collaboration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\consolidar-planilha-weg\planilas-mari-weg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456F4D28-4594-43E8-B1DD-48252D4C9F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BFC50A-5C84-48B3-953D-E87ADF6E4464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,28 +19,17 @@
     <sheet name="Jardel" sheetId="7" r:id="rId4"/>
     <sheet name="Thomas" sheetId="11" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="90">
   <si>
     <t>Epic</t>
   </si>
@@ -307,6 +296,9 @@
   </si>
   <si>
     <t>Mês 12</t>
+  </si>
+  <si>
+    <t>jan/26</t>
   </si>
 </sst>
 </file>
@@ -947,6 +939,26 @@
   </cellStyles>
   <dxfs count="241">
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC4D79B"/>
@@ -974,6 +986,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1009,6 +1028,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC5D9F1"/>
         </patternFill>
       </fill>
@@ -1021,6 +1047,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF538DD5"/>
@@ -1030,6 +1062,26 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF538DD5"/>
         </patternFill>
       </fill>
@@ -1055,12 +1107,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF538DD5"/>
@@ -1352,10 +1398,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1365,6 +1419,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC5D9F1"/>
@@ -1379,12 +1439,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF538DD5"/>
@@ -1392,6 +1446,19 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC5D9F1"/>
@@ -1406,6 +1473,26 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC4D79B"/>
@@ -1413,6 +1500,12 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF538DD5"/>
@@ -1427,10 +1520,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC4D79B"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1442,6 +1543,25 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC4D79B"/>
         </patternFill>
       </fill>
@@ -1454,10 +1574,31 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC5D9F1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1467,6 +1608,19 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF538DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFC5D9F1"/>
@@ -1476,171 +1630,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFC4D79B"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC4D79B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC5D9F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF538DD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2344,7 +2336,7 @@
     <tableColumn id="23" xr3:uid="{4421CF49-AB56-4301-BE99-45FCBA458FE9}" name="out/25" dataDxfId="194"/>
     <tableColumn id="24" xr3:uid="{F1E3BB55-ED52-4ABB-A642-0180E60B91A1}" name="nov/25" dataDxfId="193"/>
     <tableColumn id="25" xr3:uid="{C5C6F9DA-C654-4668-9412-C46C2E27CCB5}" name="dez/25" dataDxfId="192"/>
-    <tableColumn id="17" xr3:uid="{453C1F02-B3C0-420A-8706-84820C436FC0}" name="Nota" dataDxfId="191"/>
+    <tableColumn id="17" xr3:uid="{453C1F02-B3C0-420A-8706-84820C436FC0}" name="jan/26" dataDxfId="191"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3721,17 +3713,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:B30">
-    <cfRule type="expression" dxfId="102" priority="36">
-      <formula>IF(#REF!=1,1)</formula>
+    <cfRule type="expression" dxfId="102" priority="33">
+      <formula>IF($A24="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="35">
+    <cfRule type="expression" dxfId="101" priority="34">
+      <formula>IF($A24="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="35">
       <formula>IF($A24="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="34">
-      <formula>IF($A24="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="99" priority="33">
-      <formula>IF($A24="Esforço total atribuído",1)</formula>
+    <cfRule type="expression" dxfId="99" priority="36">
+      <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
@@ -3779,67 +3771,67 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24:T30">
-    <cfRule type="expression" dxfId="86" priority="20">
-      <formula>IF($B24=1,1)</formula>
+    <cfRule type="expression" dxfId="86" priority="17">
+      <formula>IF($A24="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="19">
+    <cfRule type="expression" dxfId="85" priority="18">
+      <formula>IF($A24="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="19">
       <formula>IF($A24="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="18">
-      <formula>IF($A24="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="17">
-      <formula>IF($A24="Esforço total atribuído",1)</formula>
+    <cfRule type="expression" dxfId="83" priority="20">
+      <formula>IF($B24=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O20:Q20">
-    <cfRule type="expression" dxfId="82" priority="147">
-      <formula>IF($A20="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="82" priority="145">
+      <formula>IF($A20="Esforço total atribuído",1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="81" priority="146">
       <formula>IF($A20="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="145">
-      <formula>IF($A20="Esforço total atribuído",1)</formula>
+    <cfRule type="expression" dxfId="80" priority="147">
+      <formula>IF($A20="Disponibil.total",1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="79" priority="148">
       <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23:T23">
-    <cfRule type="expression" dxfId="78" priority="139">
-      <formula>IF($A23="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="78" priority="137">
+      <formula>IF($A23="Esforço total atribuído",1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="77" priority="138">
       <formula>IF($A23="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="137">
-      <formula>IF($A23="Esforço total atribuído",1)</formula>
+    <cfRule type="expression" dxfId="76" priority="139">
+      <formula>IF($A23="Disponibil.total",1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="75" priority="140">
       <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13:Q19">
-    <cfRule type="expression" dxfId="74" priority="62">
-      <formula>IF($A13="Disponibilidade restante",1)</formula>
+    <cfRule type="expression" dxfId="74" priority="63">
+      <formula>IF($A13="Disponibil.total",1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="73" priority="61">
       <formula>IF($A13="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="63">
-      <formula>IF($A13="Disponibil.total",1)</formula>
+    <cfRule type="expression" dxfId="72" priority="62">
+      <formula>IF($A13="Disponibilidade restante",1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="71" priority="44">
       <formula>IF(#REF!=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18:Q19">
-    <cfRule type="expression" dxfId="70" priority="42">
+    <cfRule type="expression" dxfId="70" priority="43">
+      <formula>IF($A18="Disponibil.total",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="42">
       <formula>IF($A18="Disponibilidade restante",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="43">
-      <formula>IF($A18="Disponibil.total",1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="68" priority="41">
       <formula>IF($A18="Esforço total atribuído",1)</formula>
@@ -3857,9 +3849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6CD8726-B30B-4400-9738-90F4E3A3D657}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3953,7 +3945,7 @@
         <v>69</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -4100,7 +4092,9 @@
       <c r="Y3" s="21">
         <v>120</v>
       </c>
-      <c r="Z3" s="12"/>
+      <c r="Z3" s="12">
+        <v>444</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -10817,28 +10811,28 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A17:A20">
-    <cfRule type="expression" dxfId="15" priority="32">
-      <formula>IF($B17=1,1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="29">
+    <cfRule type="expression" dxfId="15" priority="29">
       <formula>IF($A17="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="30">
+    <cfRule type="expression" dxfId="14" priority="30">
       <formula>IF($A17="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="31">
+    <cfRule type="expression" dxfId="13" priority="31">
       <formula>IF($A17="Disponibil.total",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="32">
+      <formula>IF($B17=1,1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:A28">
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>IF($A22="Disponibil.total",1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>IF($A22="Esforço total atribuído",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>IF($A22="Disponibilidade restante",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>IF($A22="Disponibil.total",1)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="12">
       <formula>IF($B22=1,1)</formula>
@@ -10859,17 +10853,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:Y3">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>IF($A3="Esforço total atribuído",1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>IF($A3="Disponibilidade restante",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>IF($A3="Disponibil.total",1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>IF($B3=1,1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF($A3="Esforço total atribuído",1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -10881,17 +10875,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010055299C8A5E56DF42BB3A496FAB31A3CA" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="f48546ee30a9c08b8c56cc99cae99613">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="886f8626-7949-4fe5-8403-a629ca357b95" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4da67acbd85d4947d1135fd4f9dd5422" ns2:_="">
     <xsd:import namespace="886f8626-7949-4fe5-8403-a629ca357b95"/>
@@ -11035,31 +11018,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E1C848C-A0C9-41E4-8BB1-646104CE90D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076963EF-7E18-4286-B416-ADA05C6F6E23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="886f8626-7949-4fe5-8403-a629ca357b95"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64AD39B2-FED1-46F1-B570-2B06EBE1DD70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11077,6 +11047,30 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E1C848C-A0C9-41E4-8BB1-646104CE90D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076963EF-7E18-4286-B416-ADA05C6F6E23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="886f8626-7949-4fe5-8403-a629ca357b95"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{886666a6-a8d2-4604-a002-95b622cb7e18}" enabled="0" method="" siteId="{886666a6-a8d2-4604-a002-95b622cb7e18}" removed="1"/>

</xml_diff>